<commit_message>
Update records table columns and headers
</commit_message>
<xml_diff>
--- a/COURSE SITE DETAILS.xlsx
+++ b/COURSE SITE DETAILS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lina.ng\.gemini\antigravity\scratch\DigiApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC46E4DC-4813-47DD-A3E9-41422FC2E808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361E81F6-C43B-453F-8CD6-23C8B1FA2A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3267" uniqueCount="1064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3269" uniqueCount="1066">
   <si>
     <t>DEPT</t>
   </si>
@@ -3215,6 +3215,12 @@
   </si>
   <si>
     <t>SU4001</t>
+  </si>
+  <si>
+    <t>SOH</t>
+  </si>
+  <si>
+    <t>QET</t>
   </si>
 </sst>
 </file>
@@ -3565,10 +3571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096608EA-39C0-445C-A62C-9CA55FF5B9AB}">
-  <dimension ref="A1:C1089"/>
+  <dimension ref="A1:C1090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A1059" workbookViewId="0">
+      <selection activeCell="C1090" sqref="C1090"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -15550,6 +15556,17 @@
       </c>
       <c r="C1089" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1090" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C1090">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>